<commit_message>
Scripting botium-utterances (negations, utterance resolution, parametrization)
</commit_message>
<xml_diff>
--- a/samples/scripting/convos/xlsx/Book2.xlsx
+++ b/samples/scripting/convos/xlsx/Book2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9792" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9792"/>
   </bookViews>
   <sheets>
     <sheet name="Dialogs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>User</t>
   </si>
@@ -26,9 +26,6 @@
     <t>UTTERANCE</t>
   </si>
   <si>
-    <t>Hi</t>
-  </si>
-  <si>
     <t>Car</t>
   </si>
   <si>
@@ -41,9 +38,6 @@
     <t>hello</t>
   </si>
   <si>
-    <t>nice day</t>
-  </si>
-  <si>
     <t>where is the next restaurant</t>
   </si>
   <si>
@@ -75,6 +69,24 @@
   </si>
   <si>
     <t>super</t>
+  </si>
+  <si>
+    <t>WHERE_IS_RESTAURANT</t>
+  </si>
+  <si>
+    <t>where is a restaurant</t>
+  </si>
+  <si>
+    <t>hi, %s</t>
+  </si>
+  <si>
+    <t>hello, %s</t>
+  </si>
+  <si>
+    <t>GREETING_NAME</t>
+  </si>
+  <si>
+    <t>GREETING_NAME Bot</t>
   </si>
 </sst>
 </file>
@@ -442,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,37 +469,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
+      <c r="A4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -497,22 +509,22 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -523,13 +535,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -541,37 +557,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>